<commit_message>
update to iris petal data
</commit_message>
<xml_diff>
--- a/downloads/iris.xlsx
+++ b/downloads/iris.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipcompeau/Documents/GitHub/MMBioS/Multiscale-Biological-Modeling-Course.github.io/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D44E9728-8B48-5945-86D0-9E33D2AC2963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{230EBF58-8B88-1847-9CF5-48F12B8347E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="iris" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">iris!$C$2:$C$151</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">iris!$D$2:$D$151</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">iris!$E$2:$E$151</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">iris!$C$2:$C$151</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">iris!$D$2:$D$151</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">iris!$E$2:$E$151</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -590,6 +598,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9E2E"/>
+      <color rgb="FF8ACDF5"/>
+      <color rgb="FF36E297"/>
+      <color rgb="FFD729E6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -599,6 +615,2180 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>Petal length</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t> and width in Iris flowers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26695621646020368"/>
+          <c:y val="1.7621145374449341E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24061874431301183"/>
+          <c:y val="0.11058378715876374"/>
+          <c:w val="0.72659267909982594"/>
+          <c:h val="0.75968053002185298"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Iris setosa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D729E6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="D729E6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>iris!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>iris!$D$2:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1364-294C-A9E9-010AAED4CC0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Iris versicolor</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="36E297"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="36E297"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>iris!$C$52:$C$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>iris!$D$52:$D$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1364-294C-A9E9-010AAED4CC0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Iris virginica</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9E2E"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF9E2E"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>iris!$C$102:$C$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>iris!$D$102:$D$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1364-294C-A9E9-010AAED4CC0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="543202448"/>
+        <c:axId val="544135664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="543202448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Petal</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t> length (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1800">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544135664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="544135664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Petal width (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="543202448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.78219770299413194"/>
+          <c:y val="0.69105102500953897"/>
+          <c:w val="0.18248629749306813"/>
+          <c:h val="0.1481763155156266"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+    <a:lumOff val="20%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+    <a:lumOff val="40%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+    <a:lumOff val="30%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+    <a:lumOff val="50%"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75%"/>
+        <a:lumOff val="25%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75%"/>
+          <a:lumOff val="25%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5%"/>
+            <a:lumOff val="95%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50%"/>
+            <a:lumOff val="50%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F6846E-0AEC-7246-B5E5-8BF5E2D85329}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -900,8 +3090,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E151"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3475,5 +5665,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lots of changes to wbc conclusion and exercises
</commit_message>
<xml_diff>
--- a/downloads/iris.xlsx
+++ b/downloads/iris.xlsx
@@ -8,13 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipcompeau/Documents/GitHub/MMBioS/Multiscale-Biological-Modeling-Course.github.io/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{400F10DB-B439-0741-ACCD-19DE30165291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3BB07CE9-9D0F-C84B-87B6-276D4BC99DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1360" windowWidth="27640" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iris" sheetId="1" r:id="rId1"/>
+    <sheet name="iris_two_flowers" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">iris_two_flowers!$C$1:$D$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">iris_two_flowers!$C$2:$D$2</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">iris_two_flowers!$C$3:$D$3</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">iris_two_flowers!$C$1:$D$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">iris_two_flowers!$C$2:$D$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">iris_two_flowers!$C$3:$D$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -34,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="155" uniqueCount="8">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="162" uniqueCount="8">
   <si>
     <t>sepal_length</t>
   </si>
@@ -541,8 +550,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -655,7 +665,7 @@
                 </a:solidFill>
                 <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
               </a:rPr>
-              <a:t> and width in Iris flowers</a:t>
+              <a:t> and width in iris flowers</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="2400">
               <a:solidFill>
@@ -4658,7 +4668,7 @@
                 </a:solidFill>
                 <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
               </a:rPr>
-              <a:t> and width in Iris flowers</a:t>
+              <a:t> and width in iris flowers</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="2400">
               <a:solidFill>
@@ -6094,6 +6104,484 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0%">
+                <a:effectLst/>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>Petal length and width in iris flowers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800">
+              <a:effectLst/>
+              <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>iris_two_flowers!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>petal_width</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>iris_two_flowers!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>iris_two_flowers!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C69-8246-8119-45CD8135DAF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1348035327"/>
+        <c:axId val="1348037087"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1348035327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65%"/>
+                        <a:lumOff val="35%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400">
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Petal length (cm)</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0%">
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65%"/>
+                      <a:lumOff val="35%"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1348037087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1348037087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65%"/>
+                        <a:lumOff val="35%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400">
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>Petal width</a:t>
+                </a:r>
+                <a:br>
+                  <a:rPr lang="en-US" sz="1400">
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                </a:br>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400">
+                    <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  </a:rPr>
+                  <a:t>(cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65%"/>
+                      <a:lumOff val="35%"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Optima" panose="02000503060000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1348035327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15%"/>
+          <a:lumOff val="85%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6135,6 +6623,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+    <a:lumOff val="20%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+    <a:lumOff val="40%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+    <a:lumOff val="30%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+    <a:lumOff val="50%"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7206,6 +7734,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75%"/>
+        <a:lumOff val="25%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75%"/>
+          <a:lumOff val="25%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5%"/>
+            <a:lumOff val="95%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50%"/>
+            <a:lumOff val="50%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
   <xdr:twoCellAnchor>
@@ -7315,6 +8359,47 @@
       <a:graphic>
         <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
           <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FD195BD-4639-7245-9013-CD26E81F87C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7622,8 +8707,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="82" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A65" zoomScale="82" workbookViewId="0">
+      <selection activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10199,4 +11284,71 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7F9C41-0D32-CF49-A8EB-D648DE95E53D}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixing figure alignment chemotaxis
</commit_message>
<xml_diff>
--- a/downloads/iris.xlsx
+++ b/downloads/iris.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipcompeau/Documents/GitHub/MMBioS/Multiscale-Biological-Modeling-Course.github.io/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3BB07CE9-9D0F-C84B-87B6-276D4BC99DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{121AFF45-3D3A-184C-92EA-BA4D53B2C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1360" windowWidth="27640" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1360" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iris" sheetId="1" r:id="rId1"/>
@@ -8707,7 +8707,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="82" workbookViewId="0">
       <selection activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
@@ -11290,7 +11290,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7F9C41-0D32-CF49-A8EB-D648DE95E53D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>

</xml_diff>